<commit_message>
cambio de formato plantilla excel de productos
</commit_message>
<xml_diff>
--- a/public/files/tabla_productos.xlsx
+++ b/public/files/tabla_productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\Sitios web\AbarroteX\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8198ABDE-201F-483A-BE05-3511AC10BF6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC7521-79C5-46B0-8C45-4B327EB0937D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{841A4ED2-92B5-4BB1-8840-CAA33848FE12}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>nombre</t>
   </si>
@@ -57,6 +57,12 @@
   </si>
   <si>
     <t>stock actual</t>
+  </si>
+  <si>
+    <t>obligatorio</t>
+  </si>
+  <si>
+    <t>opcional</t>
   </si>
 </sst>
 </file>
@@ -115,10 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,14 +458,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6E9A74-4C47-4AC4-BBDB-875C92C515E2}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -469,25 +475,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizada plantilla excel para importar y actualizar indexedDB
</commit_message>
<xml_diff>
--- a/public/files/tabla_productos.xlsx
+++ b/public/files/tabla_productos.xlsx
@@ -2,74 +2,108 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Desktop\Sitios web\AbarroteX\public\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BC7521-79C5-46B0-8C45-4B327EB0937D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC6CB90-E5CB-4618-85AE-3054ECE5F015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{841A4ED2-92B5-4BB1-8840-CAA33848FE12}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
-  <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>codigo</t>
-  </si>
-  <si>
-    <t>stock minimo</t>
-  </si>
-  <si>
-    <t>precio a publico</t>
-  </si>
-  <si>
-    <t>precio de compra</t>
-  </si>
-  <si>
-    <t>stock maximo</t>
-  </si>
-  <si>
-    <t>stock actual</t>
-  </si>
-  <si>
-    <t>obligatorio</t>
-  </si>
-  <si>
-    <t>opcional</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>Precio de compra</t>
+  </si>
+  <si>
+    <t>Stock actual</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Campo obligatorio</t>
+  </si>
+  <si>
+    <t>Campo obligatorio</t>
+  </si>
+  <si>
+    <t>Es la cantidad de productos que tienes disponible en este momento</t>
+  </si>
+  <si>
+    <t>Es la cantidad máxima de productos en inventario. Previene el deterioro y la inmovilización de capital</t>
+  </si>
+  <si>
+    <t>Puedes establecer una cantidad mínima de productos que debes mantener en tu inventario</t>
+  </si>
+  <si>
+    <t>Precio que pagas al proveedor por adquirir el producto</t>
+  </si>
+  <si>
+    <t>Precio que el consumidor final paga por el producto o servicio</t>
+  </si>
+  <si>
+    <t>Campo opcional</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                      Instrucción: Ingresa los datos requeridos a partir de la</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFF68C0F"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> fila 5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFF68C0F"/>
+        <rFont val="Lato"/>
+        <family val="2"/>
+      </rPr>
+      <t>. Algunas columnas son opcionales y pueden dejarse en blanco si no tienes la información correspondiente</t>
+    </r>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Precio a publico</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Identificador único de cada producto. Puedes asignar un código propio para realizar un seguimiento interno del inventario si no cuanta con codigo de barras</t>
+  </si>
+  <si>
+    <t>Stock minimo</t>
+  </si>
+  <si>
+    <t>Stock maximo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,25 +112,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFF68C0F"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <sz val="12"/>
+      <color rgb="FFF68C0F"/>
+      <name val="Lato"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1" tint="4.9989318521683403E-2"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Lato"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="2" tint="-0.499984740745262"/>
+      <name val="Lato"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCDCB5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFF68C0F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF68C0F"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -106,14 +206,49 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFF68C0F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF68C0F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF68C0F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFF68C0F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF68C0F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF68C0F"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FFF68C0F"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FFF68C0F"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FFF68C0F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
       </bottom>
       <diagonal/>
     </border>
@@ -121,15 +256,51 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF68C0F"/>
+      <color rgb="FFFCDCB5"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -139,6 +310,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>568822</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B59BF3F-8EAF-4A9D-A4B9-66014FA8E836}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="200025" y="76200"/>
+          <a:ext cx="368797" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,70 +695,135 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E6E9A74-4C47-4AC4-BBDB-875C92C515E2}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18.600000000000001" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.109375" style="1"/>
+    <col min="9" max="9" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="21" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:13" ht="67.8" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="3"/>
+      <c r="B3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
+      <c r="D3" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="H4" s="4"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <protectedRanges>
+    <protectedRange sqref="A5:G1048576" name="Rango3"/>
+  </protectedRanges>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>